<commit_message>
Added plots for all sectors minus Others
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Schema_colors.xlsx
+++ b/TIMES_shiny/data_cleaning/Schema_colors.xlsx
@@ -1,21 +1,139 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grahamke\Documents\GitHub\TIMES-NZ\TIMES_shiny\data_cleaning\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>#447474</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>#ed6d63</t>
+  </si>
+  <si>
+    <t>Fuel Oil</t>
+  </si>
+  <si>
+    <t>#F4A28C</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>#164057</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>#41b496</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>#e94e24</t>
+  </si>
+  <si>
+    <t>LPG</t>
+  </si>
+  <si>
+    <t>#F6B3AF</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>#93B9B9</t>
+  </si>
+  <si>
+    <t>Biogas</t>
+  </si>
+  <si>
+    <t>#94DAC7</t>
+  </si>
+  <si>
+    <t>Petrol</t>
+  </si>
+  <si>
+    <t>#2a4845</t>
+  </si>
+  <si>
+    <t>Jet Fuel</t>
+  </si>
+  <si>
+    <t>#98b1c8</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>Tui</t>
+  </si>
+  <si>
+    <t>Kea</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>#02705c</t>
+  </si>
+  <si>
+    <t>Hydro</t>
+  </si>
+  <si>
+    <t>#b08204</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Waste Incineration</t>
+  </si>
+  <si>
+    <t>#382252</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>#424c69</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +181,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -109,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +267,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +302,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,191 +478,176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Fuel</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Colors</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Electric</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>#447474</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Coal</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>#ed6d63</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Fuel Oil</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>#F4A28C</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Natural Gas</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>#164057</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Wood</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>#41b496</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Diesel</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>#e94e24</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>LPG</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>#F6B3AF</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Geothermal</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>#93B9B9</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>#94DAC7</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Petrol</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>#2a4845</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Jet Fuel</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>#98b1c8</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Hydrogen</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>#579789</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Tui</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>#164057</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Kea</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>#e94e24</t>
-        </is>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Electricity to Others
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Schema_colors.xlsx
+++ b/TIMES_shiny/data_cleaning/Schema_colors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Fuel</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Coal</t>
   </si>
   <si>
-    <t>#ed6d63</t>
-  </si>
-  <si>
     <t>Fuel Oil</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>Wood</t>
   </si>
   <si>
-    <t>#41b496</t>
-  </si>
-  <si>
     <t>Diesel</t>
   </si>
   <si>
@@ -84,15 +78,9 @@
     <t>Petrol</t>
   </si>
   <si>
-    <t>#2a4845</t>
-  </si>
-  <si>
     <t>Jet Fuel</t>
   </si>
   <si>
-    <t>#98b1c8</t>
-  </si>
-  <si>
     <t>Hydrogen</t>
   </si>
   <si>
@@ -105,28 +93,46 @@
     <t>Electricity</t>
   </si>
   <si>
-    <t>#02705c</t>
-  </si>
-  <si>
     <t>Hydro</t>
   </si>
   <si>
-    <t>#b08204</t>
-  </si>
-  <si>
     <t>Solar</t>
   </si>
   <si>
     <t>Waste Incineration</t>
   </si>
   <si>
-    <t>#382252</t>
-  </si>
-  <si>
     <t>Wind</t>
   </si>
   <si>
     <t>#424c69</t>
+  </si>
+  <si>
+    <t>#ED6D63</t>
+  </si>
+  <si>
+    <t>#2A4845</t>
+  </si>
+  <si>
+    <t>#E94E24</t>
+  </si>
+  <si>
+    <t>#41B496</t>
+  </si>
+  <si>
+    <t>#FFBA6E</t>
+  </si>
+  <si>
+    <t>#FB8F71</t>
+  </si>
+  <si>
+    <t>#75C7C7</t>
+  </si>
+  <si>
+    <t>#579CB4</t>
+  </si>
+  <si>
+    <t>#8AD3FB</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +506,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -508,34 +514,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -543,79 +549,79 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,26 +634,26 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding a switch for fuel type
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Schema_colors.xlsx
+++ b/TIMES_shiny/data_cleaning/Schema_colors.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Fuel</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>#8AD3FB</t>
+  </si>
+  <si>
+    <t>Renewable</t>
+  </si>
+  <si>
+    <t>Fossil Fuel</t>
   </si>
 </sst>
 </file>
@@ -485,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,6 +662,22 @@
         <v>11</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new color schema and modified switch style
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Schema_colors.xlsx
+++ b/TIMES_shiny/data_cleaning/Schema_colors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Fuel</t>
   </si>
@@ -30,18 +30,12 @@
     <t>Electric</t>
   </si>
   <si>
-    <t>#447474</t>
-  </si>
-  <si>
     <t>Coal</t>
   </si>
   <si>
     <t>Fuel Oil</t>
   </si>
   <si>
-    <t>#F4A28C</t>
-  </si>
-  <si>
     <t>Natural Gas</t>
   </si>
   <si>
@@ -60,21 +54,12 @@
     <t>LPG</t>
   </si>
   <si>
-    <t>#F6B3AF</t>
-  </si>
-  <si>
     <t>Geothermal</t>
   </si>
   <si>
-    <t>#93B9B9</t>
-  </si>
-  <si>
     <t>Biogas</t>
   </si>
   <si>
-    <t>#94DAC7</t>
-  </si>
-  <si>
     <t>Petrol</t>
   </si>
   <si>
@@ -105,40 +90,64 @@
     <t>Wind</t>
   </si>
   <si>
-    <t>#424c69</t>
-  </si>
-  <si>
-    <t>#ED6D63</t>
-  </si>
-  <si>
-    <t>#2A4845</t>
-  </si>
-  <si>
-    <t>#E94E24</t>
-  </si>
-  <si>
-    <t>#41B496</t>
-  </si>
-  <si>
-    <t>#FFBA6E</t>
-  </si>
-  <si>
-    <t>#FB8F71</t>
-  </si>
-  <si>
-    <t>#75C7C7</t>
-  </si>
-  <si>
-    <t>#579CB4</t>
-  </si>
-  <si>
-    <t>#8AD3FB</t>
-  </si>
-  <si>
     <t>Renewable</t>
   </si>
   <si>
     <t>Fossil Fuel</t>
+  </si>
+  <si>
+    <t>#0086be</t>
+  </si>
+  <si>
+    <t>#58595b</t>
+  </si>
+  <si>
+    <t>#a7a9ac</t>
+  </si>
+  <si>
+    <t>#8a73b4</t>
+  </si>
+  <si>
+    <t>#974a21</t>
+  </si>
+  <si>
+    <t>#231f20</t>
+  </si>
+  <si>
+    <t>#f0575b</t>
+  </si>
+  <si>
+    <t>#ffc808</t>
+  </si>
+  <si>
+    <t>#4e2e8e</t>
+  </si>
+  <si>
+    <t>#c12025</t>
+  </si>
+  <si>
+    <t>#00435b</t>
+  </si>
+  <si>
+    <t>#00af8c</t>
+  </si>
+  <si>
+    <t>#6b0d0e</t>
+  </si>
+  <si>
+    <t>#53817a</t>
+  </si>
+  <si>
+    <t>#f57e20</t>
+  </si>
+  <si>
+    <t>#414042</t>
+  </si>
+  <si>
+    <t>Aviation Fuel/Kerosene</t>
+  </si>
+  <si>
+    <t>#49bee5</t>
   </si>
 </sst>
 </file>
@@ -170,7 +179,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -178,15 +187,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,191 +517,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B23" s="3" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change switch name and added hoover tip to switch
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Schema_colors.xlsx
+++ b/TIMES_shiny/data_cleaning/Schema_colors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Fuel</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Diesel</t>
-  </si>
-  <si>
-    <t>#e94e24</t>
   </si>
   <si>
     <t>LPG</t>
@@ -520,7 +517,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,42 +535,42 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -581,24 +578,24 @@
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -606,15 +603,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -622,7 +619,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,23 +627,23 @@
         <v>5</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -654,12 +651,12 @@
         <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>26</v>
@@ -670,20 +667,20 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>6</v>
@@ -691,26 +688,26 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added assumption and insight switch
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Schema_colors.xlsx
+++ b/TIMES_shiny/data_cleaning/Schema_colors.xlsx
@@ -27,9 +27,6 @@
     <t>Colors</t>
   </si>
   <si>
-    <t>Electric</t>
-  </si>
-  <si>
     <t>Coal</t>
   </si>
   <si>
@@ -141,10 +138,13 @@
     <t>#414042</t>
   </si>
   <si>
-    <t>Aviation Fuel/Kerosene</t>
-  </si>
-  <si>
     <t>#49bee5</t>
+  </si>
+  <si>
+    <t>Biodiesel</t>
+  </si>
+  <si>
+    <t>Drop-in Diesel</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,180 +534,180 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Towards code cleaning and heating/cooling calculation
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Schema_colors.xlsx
+++ b/TIMES_shiny/data_cleaning/Schema_colors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <t>Fuel</t>
   </si>
@@ -105,9 +105,6 @@
     <t>#974a21</t>
   </si>
   <si>
-    <t>#231f20</t>
-  </si>
-  <si>
     <t>#f0575b</t>
   </si>
   <si>
@@ -123,64 +120,70 @@
     <t>#00435b</t>
   </si>
   <si>
+    <t>#6b0d0e</t>
+  </si>
+  <si>
+    <t>#53817a</t>
+  </si>
+  <si>
+    <t>#f57e20</t>
+  </si>
+  <si>
+    <t>#414042</t>
+  </si>
+  <si>
+    <t>#49bee5</t>
+  </si>
+  <si>
+    <t>Biodiesel</t>
+  </si>
+  <si>
+    <t>Drop-in Diesel</t>
+  </si>
+  <si>
+    <t>Kea renewable</t>
+  </si>
+  <si>
+    <t>Tui renewable</t>
+  </si>
+  <si>
+    <t>Kea Renewable energy</t>
+  </si>
+  <si>
+    <t>Tui Renewable energy</t>
+  </si>
+  <si>
+    <t>Kea Electrification</t>
+  </si>
+  <si>
+    <t>Tui Electrification</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>triangle</t>
+  </si>
+  <si>
+    <t>circle</t>
+  </si>
+  <si>
+    <t>square</t>
+  </si>
+  <si>
+    <t>diamond</t>
+  </si>
+  <si>
+    <t>Biofuel</t>
+  </si>
+  <si>
+    <t>#35373a</t>
+  </si>
+  <si>
+    <t>#8dd2c0</t>
+  </si>
+  <si>
     <t>#00af8c</t>
-  </si>
-  <si>
-    <t>#6b0d0e</t>
-  </si>
-  <si>
-    <t>#53817a</t>
-  </si>
-  <si>
-    <t>#f57e20</t>
-  </si>
-  <si>
-    <t>#414042</t>
-  </si>
-  <si>
-    <t>#49bee5</t>
-  </si>
-  <si>
-    <t>Biodiesel</t>
-  </si>
-  <si>
-    <t>Drop-in Diesel</t>
-  </si>
-  <si>
-    <t>Kea renewable</t>
-  </si>
-  <si>
-    <t>Tui renewable</t>
-  </si>
-  <si>
-    <t>Kea Renewable energy</t>
-  </si>
-  <si>
-    <t>Tui Renewable energy</t>
-  </si>
-  <si>
-    <t>Kea Electrification</t>
-  </si>
-  <si>
-    <t>Tui Electrification</t>
-  </si>
-  <si>
-    <t>Symbol</t>
-  </si>
-  <si>
-    <t>triangle</t>
-  </si>
-  <si>
-    <t>circle</t>
-  </si>
-  <si>
-    <t>square</t>
-  </si>
-  <si>
-    <t>diamond</t>
-  </si>
-  <si>
-    <t>Biofuel</t>
   </si>
 </sst>
 </file>
@@ -555,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,7 +586,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -594,7 +597,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -605,7 +608,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,7 +619,7 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,7 +630,7 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,10 +638,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -646,10 +649,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -658,10 +661,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -669,10 +672,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,32 +683,32 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,10 +716,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -724,10 +727,10 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -735,10 +738,10 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -746,10 +749,10 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,21 +760,21 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -779,10 +782,10 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -793,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -801,10 +804,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -812,10 +815,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,76 +826,76 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Biofuel calculation for Transport
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Schema_colors.xlsx
+++ b/TIMES_shiny/data_cleaning/Schema_colors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>Fuel</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Biodiesel</t>
   </si>
   <si>
-    <t>Drop-in Diesel</t>
-  </si>
-  <si>
     <t>Kea renewable</t>
   </si>
   <si>
@@ -184,6 +181,12 @@
   </si>
   <si>
     <t>#00af8c</t>
+  </si>
+  <si>
+    <t>Drop-In Diesel</t>
+  </si>
+  <si>
+    <t>Drop-In Jet</t>
   </si>
 </sst>
 </file>
@@ -556,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -586,7 +589,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -597,7 +600,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -608,7 +611,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -619,7 +622,7 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,7 +633,7 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -638,10 +641,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,7 +655,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -664,7 +667,7 @@
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -675,7 +678,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,7 +689,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -697,15 +700,15 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>49</v>
@@ -719,7 +722,7 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,7 +733,7 @@
         <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,7 +744,7 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -752,7 +755,7 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,21 +763,21 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
         <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -785,7 +788,7 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -796,7 +799,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -804,10 +807,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -818,7 +821,7 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,76 +829,87 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Towards adding technology drilldown
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Schema_colors.xlsx
+++ b/TIMES_shiny/data_cleaning/Schema_colors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="153">
   <si>
     <t>Fuel</t>
   </si>
@@ -187,6 +187,297 @@
   </si>
   <si>
     <t>Drop-In Jet</t>
+  </si>
+  <si>
+    <t>#3E9B02</t>
+  </si>
+  <si>
+    <t>#90DA61</t>
+  </si>
+  <si>
+    <t>#3D6E1E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farm Bike                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Recovery System (Cooling)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Recovery System (Heating)       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hot Water Cylinder                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irrigator                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irrigator with VSD                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lights (General)                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refrigerator                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tractor (Agricultural)               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer Pump                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Truck (Agricultural)                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility Vehicle (Agricultural)       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vacuum Pump                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vacuum Pump with VSD                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fishing Boat (Hybrid)                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fishing Boat (Non-Hybrid)             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cable Yarder (Forestry)               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skidder (Forestry)                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stationary Motor                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boiler                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct Heat                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Pump                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biodiesel Production                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop In Bio-Jet Production            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop In Biofuel Production            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop In Diesel Production            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burner                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronics and Other Appliances      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instantaneous Water Heater           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lights (Fluorescent)                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lights (LED)                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile Motor                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistance Heater                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooking Element                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lights (Incandescent)                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oven                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEM Electrolyser                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Furnace                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal Combustion Engine            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stationary Motor with VSD             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compressor                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fan                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Exchanger                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pump                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feedstock                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrotech                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heater                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reformer                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wood/Pulp and Paper Refiner           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Pumped Storage                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithium Ion Battery                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geothermal (Consented)                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geothermal (Existing)                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro Dam (Existing)                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro Dam (New)                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro Run of River (Existing)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro Run of River (New &lt;30MW)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro Run of River (New &gt;30MW)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar (Commercial Rooftop)           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar (Existing)                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar (Grid-scale Tracking Mount)     </t>
+  </si>
+  <si>
+    <t>Combined Cycle Gas Turbine (Existing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combined Cycle Gas Turbine (New)      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combined Heat/Power                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Cycle Gas Turbine (Existing)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steam Boiler                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind (Consented)                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind (Distributed)                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind (Existing)                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind (High Capacity Factor)           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind (Low Capacity Factor)           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burner (with Wetback)                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clothes Dryer                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clothes Washer                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dishwasher                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas Heater                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Pump (Multi-Split)              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Fire                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Fire (with Wetback)              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plane                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery Electric Vehicle              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hybrid Vehicle                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plug-In Hybrid Vehicle                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ship                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geothermal (Other)                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar (Grid-scale Fixed Mount)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Cycle Gas Turbine (New)  </t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>Pumps</t>
+  </si>
+  <si>
+    <t>Generation</t>
   </si>
 </sst>
 </file>
@@ -559,15 +850,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:C31"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -697,7 +988,7 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
         <v>48</v>
@@ -708,7 +999,7 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>49</v>
@@ -906,10 +1197,1044 @@
         <v>55</v>
       </c>
       <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" t="s">
         <v>35</v>
       </c>
-      <c r="C31" t="s">
-        <v>47</v>
+      <c r="C50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>92</v>
+      </c>
+      <c r="B65" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" t="s">
+        <v>33</v>
+      </c>
+      <c r="C66" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" t="s">
+        <v>53</v>
+      </c>
+      <c r="C67" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>96</v>
+      </c>
+      <c r="B69" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70" t="s">
+        <v>23</v>
+      </c>
+      <c r="C70" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>98</v>
+      </c>
+      <c r="B71" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>102</v>
+      </c>
+      <c r="B75" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>103</v>
+      </c>
+      <c r="B76" t="s">
+        <v>28</v>
+      </c>
+      <c r="C76" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>104</v>
+      </c>
+      <c r="B77" t="s">
+        <v>34</v>
+      </c>
+      <c r="C77" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" t="s">
+        <v>30</v>
+      </c>
+      <c r="C78" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>106</v>
+      </c>
+      <c r="B79" t="s">
+        <v>31</v>
+      </c>
+      <c r="C79" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>107</v>
+      </c>
+      <c r="B80" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" t="s">
+        <v>58</v>
+      </c>
+      <c r="C81" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>109</v>
+      </c>
+      <c r="B82" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>110</v>
+      </c>
+      <c r="B83" t="s">
+        <v>37</v>
+      </c>
+      <c r="C83" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>111</v>
+      </c>
+      <c r="B84" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>112</v>
+      </c>
+      <c r="B85" t="s">
+        <v>33</v>
+      </c>
+      <c r="C85" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>113</v>
+      </c>
+      <c r="B86" t="s">
+        <v>53</v>
+      </c>
+      <c r="C86" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>114</v>
+      </c>
+      <c r="B87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>115</v>
+      </c>
+      <c r="B88" t="s">
+        <v>35</v>
+      </c>
+      <c r="C88" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>116</v>
+      </c>
+      <c r="B89" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>117</v>
+      </c>
+      <c r="B90" t="s">
+        <v>25</v>
+      </c>
+      <c r="C90" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>119</v>
+      </c>
+      <c r="B92" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>120</v>
+      </c>
+      <c r="B93" t="s">
+        <v>27</v>
+      </c>
+      <c r="C93" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>121</v>
+      </c>
+      <c r="B94" t="s">
+        <v>51</v>
+      </c>
+      <c r="C94" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>122</v>
+      </c>
+      <c r="B95" t="s">
+        <v>28</v>
+      </c>
+      <c r="C95" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>123</v>
+      </c>
+      <c r="B96" t="s">
+        <v>34</v>
+      </c>
+      <c r="C96" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>124</v>
+      </c>
+      <c r="B97" t="s">
+        <v>30</v>
+      </c>
+      <c r="C97" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>125</v>
+      </c>
+      <c r="B98" t="s">
+        <v>31</v>
+      </c>
+      <c r="C98" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>126</v>
+      </c>
+      <c r="B99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C99" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>127</v>
+      </c>
+      <c r="B100" t="s">
+        <v>58</v>
+      </c>
+      <c r="C100" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>128</v>
+      </c>
+      <c r="B101" t="s">
+        <v>32</v>
+      </c>
+      <c r="C101" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>129</v>
+      </c>
+      <c r="B102" t="s">
+        <v>37</v>
+      </c>
+      <c r="C102" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>130</v>
+      </c>
+      <c r="B103" t="s">
+        <v>29</v>
+      </c>
+      <c r="C103" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>131</v>
+      </c>
+      <c r="B104" t="s">
+        <v>33</v>
+      </c>
+      <c r="C104" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>132</v>
+      </c>
+      <c r="B105" t="s">
+        <v>53</v>
+      </c>
+      <c r="C105" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>133</v>
+      </c>
+      <c r="B106" t="s">
+        <v>32</v>
+      </c>
+      <c r="C106" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>134</v>
+      </c>
+      <c r="B107" t="s">
+        <v>35</v>
+      </c>
+      <c r="C107" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>135</v>
+      </c>
+      <c r="B108" t="s">
+        <v>23</v>
+      </c>
+      <c r="C108" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>136</v>
+      </c>
+      <c r="B109" t="s">
+        <v>25</v>
+      </c>
+      <c r="C109" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>137</v>
+      </c>
+      <c r="B110" t="s">
+        <v>24</v>
+      </c>
+      <c r="C110" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>138</v>
+      </c>
+      <c r="B111" t="s">
+        <v>26</v>
+      </c>
+      <c r="C111" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>139</v>
+      </c>
+      <c r="B112" t="s">
+        <v>27</v>
+      </c>
+      <c r="C112" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>140</v>
+      </c>
+      <c r="B113" t="s">
+        <v>51</v>
+      </c>
+      <c r="C113" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>141</v>
+      </c>
+      <c r="B114" t="s">
+        <v>28</v>
+      </c>
+      <c r="C114" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>142</v>
+      </c>
+      <c r="B115" t="s">
+        <v>34</v>
+      </c>
+      <c r="C115" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>143</v>
+      </c>
+      <c r="B116" t="s">
+        <v>30</v>
+      </c>
+      <c r="C116" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>144</v>
+      </c>
+      <c r="B117" t="s">
+        <v>31</v>
+      </c>
+      <c r="C117" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>145</v>
+      </c>
+      <c r="B118" t="s">
+        <v>56</v>
+      </c>
+      <c r="C118" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>146</v>
+      </c>
+      <c r="B119" t="s">
+        <v>58</v>
+      </c>
+      <c r="C119" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>147</v>
+      </c>
+      <c r="B120" t="s">
+        <v>32</v>
+      </c>
+      <c r="C120" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>148</v>
+      </c>
+      <c r="B121" t="s">
+        <v>34</v>
+      </c>
+      <c r="C121" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>149</v>
+      </c>
+      <c r="B122" t="s">
+        <v>30</v>
+      </c>
+      <c r="C122" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>150</v>
+      </c>
+      <c r="B123" t="s">
+        <v>31</v>
+      </c>
+      <c r="C123" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>151</v>
+      </c>
+      <c r="B124" t="s">
+        <v>56</v>
+      </c>
+      <c r="C124" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>152</v>
+      </c>
+      <c r="B125" t="s">
+        <v>32</v>
+      </c>
+      <c r="C125" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added comments to assumption plots and other fixes
</commit_message>
<xml_diff>
--- a/TIMES_shiny/data_cleaning/Schema_colors.xlsx
+++ b/TIMES_shiny/data_cleaning/Schema_colors.xlsx
@@ -60,9 +60,6 @@
     <t>Jet Fuel</t>
   </si>
   <si>
-    <t>Hydrogen</t>
-  </si>
-  <si>
     <t>Kea</t>
   </si>
   <si>
@@ -484,6 +481,9 @@
   </si>
   <si>
     <t>Tūī</t>
+  </si>
+  <si>
+    <t>Green Hydrogen</t>
   </si>
 </sst>
 </file>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,18 +875,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -894,10 +894,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -905,21 +905,21 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -927,10 +927,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -938,10 +938,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -949,10 +949,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -961,10 +961,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -972,10 +972,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -983,32 +983,32 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1016,65 +1016,65 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,1187 +1082,1187 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B67" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C67" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C69" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C72" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B73" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C73" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B74" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C74" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C75" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B76" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C76" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C77" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C78" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B79" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C79" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B80" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C80" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B81" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C81" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B82" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B83" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C83" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B84" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C84" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B85" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C85" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B86" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C86" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B87" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C87" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B88" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C88" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B89" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C89" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B90" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C90" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C91" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C92" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B93" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C93" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C94" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B95" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C95" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B96" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C96" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B97" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C97" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B98" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C98" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B99" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C99" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B100" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C100" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B101" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C101" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B102" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C102" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B103" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C103" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B104" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C104" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B105" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C105" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B106" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C106" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B107" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C107" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B108" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C108" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B109" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C109" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B110" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C110" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B111" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C111" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B112" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C112" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B113" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C113" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B114" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C114" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B115" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C115" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B116" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C116" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B117" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C117" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B118" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C118" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B119" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C119" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B120" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C120" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B121" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C121" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B122" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C122" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B123" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C123" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B124" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C124" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B125" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C125" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B126" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C126" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B127" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C127" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>